<commit_message>
journal d'abord sprint 2
</commit_message>
<xml_diff>
--- a/NelsonCuervo/Sprint2/journal d'abord Nelson Cuervo.xlsx
+++ b/NelsonCuervo/Sprint2/journal d'abord Nelson Cuervo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelson\Dropbox\PC\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelson\Dropbox\PC\Desktop\DEVELOPPEMENT-APPLICATIOS\projetChantier\NelsonCuervo\Sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725F8FD6-F2B0-42BB-A7C8-49B79A66B596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F057237B-47B7-403F-9E0A-BF9315456AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="555" windowWidth="28800" windowHeight="14655" xr2:uid="{4E6CA233-FC79-442E-BFA8-A030C94426C7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E6CA233-FC79-442E-BFA8-A030C94426C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>Nelson Alfonso Cuervo Caviedes</t>
   </si>
@@ -128,9 +120,6 @@
     <t>Meeting Equipe</t>
   </si>
   <si>
-    <t>Meeting Leonel, revision projecto</t>
-  </si>
-  <si>
     <t>Meeting Leonel, division de taches.</t>
   </si>
   <si>
@@ -144,6 +133,27 @@
   </si>
   <si>
     <t>2h30</t>
+  </si>
+  <si>
+    <t>Meeting Leonel, revision projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1h </t>
+  </si>
+  <si>
+    <t>Meeting avec le equipe.</t>
+  </si>
+  <si>
+    <t>Avancement du codage, ecriture et modificacion des utilites de la app Chantier</t>
+  </si>
+  <si>
+    <t>6h30</t>
+  </si>
+  <si>
+    <t>Meeting Equipe : état d`avancement finalisation du projet et discussion des différents points à présenter au professeur</t>
+  </si>
+  <si>
+    <t>30 min</t>
   </si>
 </sst>
 </file>
@@ -179,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -191,6 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,7 +508,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -505,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72050F50-CF0C-4E9B-ADE3-1D6CB7D01C36}">
-  <dimension ref="B4:E32"/>
+  <dimension ref="B4:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,7 +704,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>7</v>
       </c>
@@ -707,7 +718,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>8</v>
       </c>
@@ -757,7 +768,7 @@
         <v>44924</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E29" t="s">
         <v>4</v>
@@ -771,7 +782,7 @@
         <v>44925</v>
       </c>
       <c r="D30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
@@ -779,27 +790,91 @@
         <v>13</v>
       </c>
       <c r="C31" s="1">
-        <v>44935</v>
+        <v>44929</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E31" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C32" s="1">
+        <v>44935</v>
+      </c>
+      <c r="D32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="2">
+        <v>15</v>
+      </c>
+      <c r="C33" s="1">
         <v>44936</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" t="s">
         <v>35</v>
       </c>
-      <c r="E32" t="s">
-        <v>36</v>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="2">
+        <v>16</v>
+      </c>
+      <c r="C34" s="5">
+        <v>44940</v>
+      </c>
+      <c r="D34" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="2">
+        <v>17</v>
+      </c>
+      <c r="C36" s="5">
+        <v>44941</v>
+      </c>
+      <c r="D36" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>18</v>
+      </c>
+      <c r="C37" s="5">
+        <v>44942</v>
+      </c>
+      <c r="D37" t="s">
+        <v>41</v>
+      </c>
+      <c r="E37" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>